<commit_message>
Modified Terrain and began working on Fight Logic
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\repo\GalactiPandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{072D7618-CCC9-4F17-AAC4-D457DD171093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89900D0-1D4D-42BE-8358-CA579670E36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{AEA0231A-B28A-4A53-9AE7-96D188979516}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
   <si>
     <t>#</t>
   </si>
@@ -215,6 +215,87 @@
   </si>
   <si>
     <t>1.2.6</t>
+  </si>
+  <si>
+    <t>Worker</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Volcano</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Glacier</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
+  </si>
+  <si>
+    <t>1.5.4</t>
+  </si>
+  <si>
+    <t>1.5.5</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>Combat</t>
+  </si>
+  <si>
+    <t>Shop (Speech)</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>1.5.6</t>
+  </si>
+  <si>
+    <t>Speech</t>
   </si>
 </sst>
 </file>
@@ -279,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -289,12 +370,19 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -327,16 +415,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B432282D-C3E0-459C-B678-13E21099B9DB}" name="Table1" displayName="Table1" ref="A1:G38" totalsRowShown="0">
-  <autoFilter ref="A1:G38" xr:uid="{B432282D-C3E0-459C-B678-13E21099B9DB}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9C9D192A-59BD-4AAD-8C5D-59E4925F5397}" name="#" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{71A679AA-46E8-47D9-A707-4A3C3F40133D}" name="Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CA9CDE85-DF37-43AE-BFF0-6995BE6AEFE0}" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FC714E55-39BE-4706-89A8-D3580CB148CD}" name="Date Started" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{2A890283-9922-4C92-B805-CE7C0EACAD23}" name="Date Completed" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{CDB4868D-3C4F-4EED-AF95-7E7C4022803E}" name="Due Date" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B432282D-C3E0-459C-B678-13E21099B9DB}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0">
+  <autoFilter ref="A1:H49" xr:uid="{B432282D-C3E0-459C-B678-13E21099B9DB}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9C9D192A-59BD-4AAD-8C5D-59E4925F5397}" name="#" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{71A679AA-46E8-47D9-A707-4A3C3F40133D}" name="Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{CA9CDE85-DF37-43AE-BFF0-6995BE6AEFE0}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{FC714E55-39BE-4706-89A8-D3580CB148CD}" name="Date Started" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2A890283-9922-4C92-B805-CE7C0EACAD23}" name="Date Completed" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CDB4868D-3C4F-4EED-AF95-7E7C4022803E}" name="Due Date" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{14F20077-EAF9-4FC1-B3E0-DAE4EA2B317A}" name="Status" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{ABB9D171-24ED-43E6-AA64-B5F9056A9404}" name="Worker" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -639,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614E4CC4-4F23-4ED1-8022-48E09316191D}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +767,9 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
@@ -694,7 +786,7 @@
         <f>AVERAGE(G3:G27)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -711,6 +803,9 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -726,6 +821,9 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -741,6 +839,9 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -756,6 +857,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -768,7 +870,12 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -781,7 +888,12 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -794,7 +906,12 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -807,7 +924,12 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -820,7 +942,12 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -833,7 +960,12 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -849,6 +981,7 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -864,6 +997,9 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
+      <c r="H14" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -879,6 +1015,9 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
+      <c r="H15" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -894,8 +1033,11 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -909,8 +1051,11 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -924,8 +1069,11 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -939,8 +1087,11 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -954,8 +1105,9 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -969,8 +1121,11 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -984,8 +1139,11 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -999,8 +1157,11 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
@@ -1014,8 +1175,11 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -1029,8 +1193,11 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -1044,8 +1211,11 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -1059,118 +1229,140 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="H27" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>2</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="10">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>2.1</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="2"/>
@@ -1179,28 +1371,34 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>4</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>4.0999999999999996</v>
+      <c r="H35" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="2"/>
@@ -1209,25 +1407,225 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="H37" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="10">
+        <v>0</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>3</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>4</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>4.2</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="1">
-        <v>0</v>
+      <c r="C49" s="3"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="percent" val="0"/>

</xml_diff>